<commit_message>
Day 4  - Email Automation
</commit_message>
<xml_diff>
--- a/Input/Rules.xlsx
+++ b/Input/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahil\OneDrive - RPATech\Desktop\Final for Reference\New folder\Lesson 4\4.3.1 Email Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simmi Anand\Documents\UiPath\First Process 120165\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC6DAA7-717B-4809-ACFE-516E4563D1B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B7B42F-16A1-4CC1-B150-E29FA54B2A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2136" yWindow="3168" windowWidth="14892" windowHeight="7500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>github.com</t>
   </si>
   <si>
-    <t>Google.com</t>
-  </si>
-  <si>
     <t>Google</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>google.com</t>
   </si>
 </sst>
 </file>
@@ -410,15 +410,15 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,23 +426,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -450,12 +450,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -464,34 +464,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="b7a32e9a-83ed-4fc1-afd2-24748cc0fd29">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="1103b93a-9ee9-47ae-aa92-e31c5ef9a1ca" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1103b93a-9ee9-47ae-aa92-e31c5ef9a1ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b7a32e9a-83ed-4fc1-afd2-24748cc0fd29" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100640219CDDE981245A35CC9C2134D8B03" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4b6277c6e191b84b85c9c8695654794d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1103b93a-9ee9-47ae-aa92-e31c5ef9a1ca" xmlns:ns3="b7a32e9a-83ed-4fc1-afd2-24748cc0fd29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="126733d01f79f7f731e3d21e095d20f3" ns2:_="" ns3:_="">
     <xsd:import namespace="1103b93a-9ee9-47ae-aa92-e31c5ef9a1ca"/>
@@ -722,11 +694,49 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="b7a32e9a-83ed-4fc1-afd2-24748cc0fd29">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="1103b93a-9ee9-47ae-aa92-e31c5ef9a1ca" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1103b93a-9ee9-47ae-aa92-e31c5ef9a1ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b7a32e9a-83ed-4fc1-afd2-24748cc0fd29" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1776547D-6BF6-48C7-ADED-07CD3E5E3AF3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4841C1-90A0-4487-96EA-A92E4E4DA23A}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1103b93a-9ee9-47ae-aa92-e31c5ef9a1ca"/>
+    <ds:schemaRef ds:uri="b7a32e9a-83ed-4fc1-afd2-24748cc0fd29"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -740,5 +750,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4841C1-90A0-4487-96EA-A92E4E4DA23A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1776547D-6BF6-48C7-ADED-07CD3E5E3AF3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b7a32e9a-83ed-4fc1-afd2-24748cc0fd29"/>
+    <ds:schemaRef ds:uri="1103b93a-9ee9-47ae-aa92-e31c5ef9a1ca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>